<commit_message>
Extend the capabilities of Data driven approach
</commit_message>
<xml_diff>
--- a/Run Manager.xlsx
+++ b/Run Manager.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>SalesPage_TC4</t>
+  </si>
+  <si>
+    <t>LoginPage</t>
   </si>
 </sst>
 </file>
@@ -169,21 +172,21 @@
   <dxfs count="4">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -486,7 +489,7 @@
   <dimension ref="A1:Q113"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +524,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -955,10 +958,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed few issues with Extent reports and added DB handler
</commit_message>
<xml_diff>
--- a/Run Manager.xlsx
+++ b/Run Manager.xlsx
@@ -45,9 +45,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>LoginPage</t>
+  </si>
+  <si>
+    <t>CHROME</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:Q113"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,22 +524,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -547,119 +547,119 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -672,22 +672,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -945,11 +945,11 @@
     </row>
     <row r="113" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q113" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D9 D11:D1048576">
+  <conditionalFormatting sqref="D11:D1048576 D1:D9">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>

</xml_diff>